<commit_message>
All documentation is added
</commit_message>
<xml_diff>
--- a/Results /ml_codes_results.xlsx
+++ b/Results /ml_codes_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Results /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEBACCB-8F01-8045-B504-46D7C08164B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA5E980-2426-8742-9443-08FE69A2D3FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="100">
   <si>
     <t>Negative DES</t>
   </si>
@@ -243,21 +243,9 @@
     <t>0.97325</t>
   </si>
   <si>
-    <t>36.93292495435067</t>
-  </si>
-  <si>
-    <t>5.149189540418116</t>
-  </si>
-  <si>
     <t>0.648936170212766</t>
   </si>
   <si>
-    <t>41.08357046696423</t>
-  </si>
-  <si>
-    <t>4.701363590128555</t>
-  </si>
-  <si>
     <t>0.48214285714285715</t>
   </si>
   <si>
@@ -304,6 +292,48 @@
   </si>
   <si>
     <t xml:space="preserve">hidden_layer_sizes = (1000, 100, 100), </t>
+  </si>
+  <si>
+    <t>0.9999999999999972</t>
+  </si>
+  <si>
+    <t>0.9735</t>
+  </si>
+  <si>
+    <t>1.0011445448948948</t>
+  </si>
+  <si>
+    <t>0.00045433046323221205</t>
+  </si>
+  <si>
+    <t>1.0004165781795227</t>
+  </si>
+  <si>
+    <t>0.0001933158743593073</t>
+  </si>
+  <si>
+    <t>0.5059523809523809</t>
+  </si>
+  <si>
+    <t>0.00011520733270134534</t>
+  </si>
+  <si>
+    <t>1.0004686821963849</t>
+  </si>
+  <si>
+    <t>0.5458015267175572</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hidden_layer_sizes = (100, 100), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">solver = 'adam', </t>
+  </si>
+  <si>
+    <t>verbose = True,</t>
+  </si>
+  <si>
+    <t>max_iter = 100)</t>
   </si>
 </sst>
 </file>
@@ -784,19 +814,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
@@ -811,13 +835,126 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -826,95 +963,56 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -922,82 +1020,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1321,795 +1354,980 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06CD785-33B7-3045-A313-C2EB4D15E3B6}">
   <dimension ref="A1:AO29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AN15" sqref="AN15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" style="38" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.1640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6" style="39" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.33203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.83203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.33203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.5" style="38" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="15" style="38" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15" style="58" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.83203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.1640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="15" style="38" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.83203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.83203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.5" style="38" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.33203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.33203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.83203125" style="62" bestFit="1" customWidth="1"/>
-    <col min="41" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="12.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6" style="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.83203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" style="26" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15" style="41" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.83203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.83203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="41" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="71" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:41" s="51" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
-    </row>
-    <row r="2" spans="1:41" s="71" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="72"/>
-      <c r="B2" s="73" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+    </row>
+    <row r="2" spans="1:41" s="51" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="71"/>
+      <c r="B2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="70"/>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="70"/>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="70"/>
-      <c r="AF2" s="70"/>
-      <c r="AG2" s="70"/>
-    </row>
-    <row r="3" spans="1:41" s="71" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="67" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="50"/>
+      <c r="AD2" s="50"/>
+      <c r="AE2" s="50"/>
+      <c r="AF2" s="50"/>
+      <c r="AG2" s="50"/>
+    </row>
+    <row r="3" spans="1:41" s="51" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="70"/>
-      <c r="AC3" s="70"/>
-      <c r="AD3" s="70"/>
-      <c r="AE3" s="70"/>
-      <c r="AF3" s="70"/>
-      <c r="AG3" s="70"/>
-    </row>
-    <row r="4" spans="1:41" s="71" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="75"/>
-      <c r="B4" s="76" t="s">
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50"/>
+      <c r="AA3" s="50"/>
+      <c r="AB3" s="50"/>
+      <c r="AC3" s="50"/>
+      <c r="AD3" s="50"/>
+      <c r="AE3" s="50"/>
+      <c r="AF3" s="50"/>
+      <c r="AG3" s="50"/>
+    </row>
+    <row r="4" spans="1:41" s="51" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="72"/>
+      <c r="B4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70" t="s">
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="70"/>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
-      <c r="U4" s="70"/>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
-      <c r="AB4" s="70"/>
-      <c r="AC4" s="70"/>
-      <c r="AD4" s="70"/>
-      <c r="AE4" s="70"/>
-      <c r="AF4" s="70"/>
-      <c r="AG4" s="70"/>
-    </row>
-    <row r="5" spans="1:41" s="71" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="78"/>
-      <c r="B5" s="73" t="s">
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="50"/>
+      <c r="AA4" s="50"/>
+      <c r="AB4" s="50"/>
+      <c r="AC4" s="50"/>
+      <c r="AD4" s="50"/>
+      <c r="AE4" s="50"/>
+      <c r="AF4" s="50"/>
+      <c r="AG4" s="50"/>
+    </row>
+    <row r="5" spans="1:41" s="51" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="73"/>
+      <c r="B5" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70" t="s">
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="70"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="70"/>
-      <c r="AB5" s="70"/>
-      <c r="AC5" s="70"/>
-      <c r="AD5" s="70"/>
-      <c r="AE5" s="70"/>
-      <c r="AF5" s="70"/>
-      <c r="AG5" s="70"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
+      <c r="T5" s="50"/>
+      <c r="U5" s="50"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="50"/>
+      <c r="X5" s="50"/>
+      <c r="Y5" s="50"/>
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="50"/>
+      <c r="AB5" s="50"/>
+      <c r="AC5" s="50"/>
+      <c r="AD5" s="50"/>
+      <c r="AE5" s="50"/>
+      <c r="AF5" s="50"/>
+      <c r="AG5" s="50"/>
     </row>
     <row r="6" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="14"/>
-      <c r="AI6" s="14"/>
-      <c r="AJ6" s="14"/>
-      <c r="AK6" s="14"/>
-      <c r="AL6" s="14"/>
-      <c r="AM6" s="14"/>
-      <c r="AN6" s="14"/>
-      <c r="AO6" s="15"/>
-    </row>
-    <row r="7" spans="1:41" s="29" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="12"/>
+      <c r="AI6" s="12"/>
+      <c r="AJ6" s="12"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="12"/>
+      <c r="AM6" s="12"/>
+      <c r="AN6" s="12"/>
+      <c r="AO6" s="13"/>
+    </row>
+    <row r="7" spans="1:41" s="19" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19" t="s">
+      <c r="E7" s="67"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21" t="s">
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="23" t="s">
+      <c r="K7" s="57"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="24" t="s">
+      <c r="N7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="O7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="P7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" s="25" t="s">
+      <c r="Q7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="S7" s="57" t="s">
+      <c r="S7" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="T7" s="26" t="s">
+      <c r="T7" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="6" t="s">
+      <c r="U7" s="65"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="60" t="s">
+      <c r="X7" s="60"/>
+      <c r="Y7" s="60"/>
+      <c r="Z7" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="AA7" s="19" t="s">
+      <c r="AA7" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="20"/>
-      <c r="AC7" s="50"/>
-      <c r="AD7" s="27" t="s">
+      <c r="AB7" s="57"/>
+      <c r="AC7" s="58"/>
+      <c r="AD7" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="AE7" s="27"/>
-      <c r="AF7" s="27"/>
-      <c r="AG7" s="60" t="s">
+      <c r="AE7" s="17"/>
+      <c r="AF7" s="17"/>
+      <c r="AG7" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="AH7" s="19" t="s">
+      <c r="AH7" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="AI7" s="20"/>
-      <c r="AJ7" s="50"/>
-      <c r="AK7" s="19" t="s">
+      <c r="AI7" s="57"/>
+      <c r="AJ7" s="58"/>
+      <c r="AK7" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="AL7" s="20"/>
-      <c r="AM7" s="50"/>
-      <c r="AN7" s="60" t="s">
+      <c r="AL7" s="57"/>
+      <c r="AM7" s="58"/>
+      <c r="AN7" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="AO7" s="28"/>
+      <c r="AO7" s="18"/>
     </row>
     <row r="8" spans="1:41" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="30">
+      <c r="A8" s="61">
         <v>1</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="35" t="s">
+      <c r="N8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="35" t="s">
+      <c r="O8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="Q8" s="33" t="s">
+      <c r="Q8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="R8" s="46"/>
-      <c r="T8" s="36" t="s">
+      <c r="R8" s="33"/>
+      <c r="T8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="U8" s="36" t="s">
+      <c r="U8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="V8" s="36" t="s">
+      <c r="V8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="W8" s="36" t="s">
+      <c r="W8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="X8" s="36" t="s">
+      <c r="X8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="Y8" s="36" t="s">
+      <c r="Y8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="49" t="s">
+      <c r="Z8" s="44"/>
+      <c r="AA8" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="AB8" s="36" t="s">
+      <c r="AB8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="AC8" s="36" t="s">
+      <c r="AC8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AD8" s="36" t="s">
+      <c r="AD8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="AE8" s="36" t="s">
+      <c r="AE8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="AF8" s="36" t="s">
+      <c r="AF8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AG8" s="61"/>
-      <c r="AH8" s="36" t="s">
+      <c r="AG8" s="44"/>
+      <c r="AH8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="AI8" s="36" t="s">
+      <c r="AI8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="AJ8" s="36" t="s">
+      <c r="AJ8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AK8" s="35" t="s">
+      <c r="AK8" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AL8" s="33" t="s">
+      <c r="AL8" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="AM8" s="35" t="s">
+      <c r="AM8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="AN8" s="63"/>
+      <c r="AN8" s="46"/>
     </row>
     <row r="9" spans="1:41" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
-      <c r="B9" s="65" t="s">
+      <c r="A9" s="62"/>
+      <c r="B9" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Y9" s="48"/>
-      <c r="Z9" s="62"/>
-      <c r="AA9" s="39"/>
-      <c r="AB9" s="13"/>
-      <c r="AG9" s="62"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="45"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="11"/>
+      <c r="AG9" s="45"/>
     </row>
     <row r="10" spans="1:41" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
-      <c r="B10" s="65" t="s">
+      <c r="A10" s="62"/>
+      <c r="B10" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="38" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="26">
+        <v>20000</v>
+      </c>
+      <c r="N10" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="O10" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="P10" s="27">
+        <v>16000</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>4000</v>
+      </c>
+      <c r="R10" s="26">
+        <v>49</v>
+      </c>
+      <c r="S10" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="T10" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="U10" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="V10" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="W10" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="X10" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y10" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z10" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA10" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB10" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC10" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD10" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE10" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF10" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG10" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH10" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI10" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="J10" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="M10" s="38">
-        <v>20000</v>
-      </c>
-      <c r="N10" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="O10" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="P10" s="39">
-        <v>16000</v>
-      </c>
-      <c r="Q10" s="38">
-        <v>4000</v>
-      </c>
-      <c r="R10" s="38">
-        <v>49</v>
-      </c>
-      <c r="S10" s="58" t="s">
+      <c r="AJ10" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="T10" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="U10" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="V10" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="W10" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="X10" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y10" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z10" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA10" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB10" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC10" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD10" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE10" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF10" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG10" s="58" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH10" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI10" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ10" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK10" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL10" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM10" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN10" s="62" t="s">
-        <v>88</v>
+      <c r="AK10" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL10" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM10" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN10" s="45" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:41" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="65" t="s">
+      <c r="A11" s="62"/>
+      <c r="B11" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:41" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
-      <c r="B12" s="66" t="s">
+      <c r="A12" s="63"/>
+      <c r="B12" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="59"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="42"/>
-      <c r="X12" s="42"/>
-      <c r="Y12" s="42"/>
-      <c r="Z12" s="59"/>
-      <c r="AA12" s="42"/>
-      <c r="AB12" s="42"/>
-      <c r="AC12" s="42"/>
-      <c r="AD12" s="42"/>
-      <c r="AE12" s="42"/>
-      <c r="AF12" s="42"/>
-      <c r="AG12" s="59"/>
-      <c r="AH12" s="42"/>
-      <c r="AI12" s="42"/>
-      <c r="AJ12" s="42"/>
-      <c r="AK12" s="42"/>
-      <c r="AL12" s="42"/>
-      <c r="AM12" s="43"/>
-      <c r="AN12" s="64"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="29"/>
+      <c r="X12" s="29"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="42"/>
+      <c r="AA12" s="29"/>
+      <c r="AB12" s="29"/>
+      <c r="AC12" s="29"/>
+      <c r="AD12" s="29"/>
+      <c r="AE12" s="29"/>
+      <c r="AF12" s="29"/>
+      <c r="AG12" s="42"/>
+      <c r="AH12" s="29"/>
+      <c r="AI12" s="29"/>
+      <c r="AJ12" s="29"/>
+      <c r="AK12" s="29"/>
+      <c r="AL12" s="29"/>
+      <c r="AM12" s="30"/>
+      <c r="AN12" s="47"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A13" s="44">
+      <c r="A13" s="31">
         <v>2</v>
       </c>
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="80" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="B15" s="80" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M15" s="26">
+        <v>20000</v>
+      </c>
+      <c r="N15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="O15" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="P15" s="27">
+        <v>16000</v>
+      </c>
+      <c r="Q15" s="26">
+        <v>4000</v>
+      </c>
+      <c r="R15" s="26">
+        <v>28</v>
+      </c>
+      <c r="S15" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="T15" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="U15" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="V15" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="W15" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="X15" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="Y15" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z15" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA15" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB15" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC15" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD15" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE15" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF15" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG15" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH15" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI15" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ15" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK15" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL15" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM15" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN15" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="B16" s="80" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="42"/>
+      <c r="AA17" s="29"/>
+      <c r="AB17" s="29"/>
+      <c r="AC17" s="29"/>
+      <c r="AD17" s="29"/>
+      <c r="AE17" s="29"/>
+      <c r="AF17" s="29"/>
+      <c r="AG17" s="42"/>
+      <c r="AH17" s="29"/>
+      <c r="AI17" s="29"/>
+      <c r="AJ17" s="29"/>
+      <c r="AK17" s="29"/>
+      <c r="AL17" s="29"/>
+      <c r="AM17" s="30"/>
+      <c r="AN17" s="47"/>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A18" s="12">
+        <v>3</v>
+      </c>
+      <c r="B18" s="80" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B19" s="80" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="B15" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="13"/>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="B16" s="79" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="13" t="s">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B20" s="80" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="80" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:40" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="80" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="59"/>
-      <c r="T17" s="42"/>
-      <c r="U17" s="42"/>
-      <c r="V17" s="42"/>
-      <c r="W17" s="42"/>
-      <c r="X17" s="42"/>
-      <c r="Y17" s="42"/>
-      <c r="Z17" s="59"/>
-      <c r="AA17" s="42"/>
-      <c r="AB17" s="42"/>
-      <c r="AC17" s="42"/>
-      <c r="AD17" s="42"/>
-      <c r="AE17" s="42"/>
-      <c r="AF17" s="42"/>
-      <c r="AG17" s="59"/>
-      <c r="AH17" s="42"/>
-      <c r="AI17" s="42"/>
-      <c r="AJ17" s="42"/>
-      <c r="AK17" s="42"/>
-      <c r="AL17" s="42"/>
-      <c r="AM17" s="43"/>
-      <c r="AN17" s="64"/>
-    </row>
-    <row r="21" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:40" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="29"/>
+      <c r="X22" s="29"/>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="42"/>
+      <c r="AA22" s="29"/>
+      <c r="AB22" s="29"/>
+      <c r="AC22" s="29"/>
+      <c r="AD22" s="29"/>
+      <c r="AE22" s="29"/>
+      <c r="AF22" s="29"/>
+      <c r="AG22" s="42"/>
+      <c r="AH22" s="29"/>
+      <c r="AI22" s="29"/>
+      <c r="AJ22" s="29"/>
+      <c r="AK22" s="29"/>
+      <c r="AL22" s="29"/>
+      <c r="AM22" s="30"/>
+      <c r="AN22" s="47"/>
+    </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="45"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="32"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="45"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="32"/>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="45"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="32"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="45"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="32"/>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="45"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="N4:S4"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="AH7:AJ7"/>
     <mergeCell ref="AK7:AM7"/>
     <mergeCell ref="W7:Y7"/>
@@ -2119,8 +2337,6 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2128,10 +2344,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974E9989-1B5F-FF41-9AD2-81024DE4B8DD}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2146,31 +2362,31 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="75"/>
+      <c r="F1" s="76"/>
+    </row>
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-    </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2184,13 +2400,33 @@
         <v>68</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This is updating the results
</commit_message>
<xml_diff>
--- a/Results /ml_codes_results.xlsx
+++ b/Results /ml_codes_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Results /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA5E980-2426-8742-9443-08FE69A2D3FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AD305A-0964-C54F-9393-5C829A9E15B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="106">
   <si>
     <t>Negative DES</t>
   </si>
@@ -334,13 +334,31 @@
   </si>
   <si>
     <t>max_iter = 100)</t>
+  </si>
+  <si>
+    <t>0.96575</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.0002863525717804</t>
+  </si>
+  <si>
+    <t>0.6595744680851063</t>
+  </si>
+  <si>
+    <t>0.5297619047619048</t>
+  </si>
+  <si>
+    <t>0.5687022900763359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hidden_layer_sizes = (1000, 100), </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -364,21 +382,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -814,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -835,40 +840,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -889,27 +894,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -918,58 +920,34 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -981,35 +959,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1020,9 +986,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1031,6 +994,39 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1354,15 +1350,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06CD785-33B7-3045-A313-C2EB4D15E3B6}">
   <dimension ref="A1:AO29"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AN15" sqref="AN15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="30.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.1640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="32.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
@@ -1378,178 +1374,175 @@
     <col min="16" max="16" width="6" style="27" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.83203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.83203125" style="40" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.5" style="26" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15" style="26" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15" style="41" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15" style="40" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="18.1640625" style="26" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10.6640625" style="26" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.5" style="26" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.83203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.83203125" style="40" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="19.6640625" style="26" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="11.5" style="26" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="19.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.83203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.83203125" style="44" bestFit="1" customWidth="1"/>
     <col min="41" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="51" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:41" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="50"/>
-      <c r="AD1" s="50"/>
-      <c r="AE1" s="50"/>
-      <c r="AF1" s="50"/>
-      <c r="AG1" s="50"/>
-    </row>
-    <row r="2" spans="1:41" s="51" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+    </row>
+    <row r="2" spans="1:41" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="71"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="50"/>
-      <c r="AC2" s="50"/>
-      <c r="AD2" s="50"/>
-      <c r="AE2" s="50"/>
-      <c r="AF2" s="50"/>
-      <c r="AG2" s="50"/>
-    </row>
-    <row r="3" spans="1:41" s="51" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="70" t="s">
+      <c r="G2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+    </row>
+    <row r="3" spans="1:41" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
-      <c r="Y3" s="50"/>
-      <c r="Z3" s="50"/>
-      <c r="AA3" s="50"/>
-      <c r="AB3" s="50"/>
-      <c r="AC3" s="50"/>
-      <c r="AD3" s="50"/>
-      <c r="AE3" s="50"/>
-      <c r="AF3" s="50"/>
-      <c r="AG3" s="50"/>
-    </row>
-    <row r="4" spans="1:41" s="51" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="72"/>
-      <c r="B4" s="54" t="s">
+      <c r="G3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="12"/>
+      <c r="AI3" s="12"/>
+      <c r="AJ3" s="12"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="12"/>
+      <c r="AM3" s="12"/>
+      <c r="AN3" s="12"/>
+    </row>
+    <row r="4" spans="1:41" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="74"/>
+      <c r="B4" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
+      <c r="G4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="M4" s="11"/>
       <c r="N4" s="77" t="s">
         <v>65</v>
       </c>
@@ -1558,63 +1551,71 @@
       <c r="Q4" s="77"/>
       <c r="R4" s="77"/>
       <c r="S4" s="77"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50"/>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="50"/>
-      <c r="Z4" s="50"/>
-      <c r="AA4" s="50"/>
-      <c r="AB4" s="50"/>
-      <c r="AC4" s="50"/>
-      <c r="AD4" s="50"/>
-      <c r="AE4" s="50"/>
-      <c r="AF4" s="50"/>
-      <c r="AG4" s="50"/>
-    </row>
-    <row r="5" spans="1:41" s="51" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="73"/>
-      <c r="B5" s="52" t="s">
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="12"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="12"/>
+    </row>
+    <row r="5" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="78"/>
+      <c r="B5" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
+      <c r="G5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="M5" s="11"/>
       <c r="N5" s="77" t="s">
         <v>66</v>
       </c>
       <c r="O5" s="77"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="50"/>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
-      <c r="AB5" s="50"/>
-      <c r="AC5" s="50"/>
-      <c r="AD5" s="50"/>
-      <c r="AE5" s="50"/>
-      <c r="AF5" s="50"/>
-      <c r="AG5" s="50"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="12"/>
+      <c r="AJ5" s="12"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="12"/>
     </row>
     <row r="6" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
@@ -1655,97 +1656,97 @@
       <c r="AO6" s="13"/>
     </row>
     <row r="7" spans="1:41" s="19" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="D7" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="56" t="s">
+      <c r="E7" s="58"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="69" t="s">
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="57"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="14" t="s">
+      <c r="K7" s="48"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="15" t="s">
+      <c r="N7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="P7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="34" t="s">
+      <c r="R7" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="S7" s="40" t="s">
+      <c r="S7" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="T7" s="64" t="s">
+      <c r="T7" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="65"/>
-      <c r="V7" s="65"/>
-      <c r="W7" s="59" t="s">
+      <c r="U7" s="56"/>
+      <c r="V7" s="56"/>
+      <c r="W7" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="60"/>
-      <c r="Z7" s="43" t="s">
+      <c r="X7" s="51"/>
+      <c r="Y7" s="51"/>
+      <c r="Z7" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="AA7" s="56" t="s">
+      <c r="AA7" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="57"/>
-      <c r="AC7" s="58"/>
+      <c r="AB7" s="48"/>
+      <c r="AC7" s="49"/>
       <c r="AD7" s="17" t="s">
         <v>63</v>
       </c>
       <c r="AE7" s="17"/>
       <c r="AF7" s="17"/>
-      <c r="AG7" s="43" t="s">
+      <c r="AG7" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="AH7" s="56" t="s">
+      <c r="AH7" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="AI7" s="57"/>
-      <c r="AJ7" s="58"/>
-      <c r="AK7" s="56" t="s">
+      <c r="AI7" s="48"/>
+      <c r="AJ7" s="49"/>
+      <c r="AK7" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="AL7" s="57"/>
-      <c r="AM7" s="58"/>
-      <c r="AN7" s="43" t="s">
+      <c r="AL7" s="48"/>
+      <c r="AM7" s="49"/>
+      <c r="AN7" s="42" t="s">
         <v>23</v>
       </c>
       <c r="AO7" s="18"/>
     </row>
     <row r="8" spans="1:41" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="61">
+      <c r="A8" s="52">
         <v>1</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="64" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -1793,7 +1794,7 @@
       <c r="Q8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="R8" s="33"/>
+      <c r="R8" s="32"/>
       <c r="T8" s="25" t="s">
         <v>43</v>
       </c>
@@ -1812,8 +1813,8 @@
       <c r="Y8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="Z8" s="44"/>
-      <c r="AA8" s="36" t="s">
+      <c r="Z8" s="43"/>
+      <c r="AA8" s="35" t="s">
         <v>43</v>
       </c>
       <c r="AB8" s="25" t="s">
@@ -1831,7 +1832,7 @@
       <c r="AF8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AG8" s="44"/>
+      <c r="AG8" s="43"/>
       <c r="AH8" s="25" t="s">
         <v>43</v>
       </c>
@@ -1850,25 +1851,25 @@
       <c r="AM8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="AN8" s="46"/>
+      <c r="AN8" s="45"/>
     </row>
     <row r="9" spans="1:41" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="62"/>
-      <c r="B9" s="78" t="s">
+      <c r="A9" s="53"/>
+      <c r="B9" s="64" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Y9" s="35"/>
-      <c r="Z9" s="45"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="44"/>
       <c r="AA9" s="27"/>
       <c r="AB9" s="11"/>
-      <c r="AG9" s="45"/>
+      <c r="AG9" s="44"/>
     </row>
     <row r="10" spans="1:41" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="62"/>
-      <c r="B10" s="78" t="s">
+      <c r="A10" s="53"/>
+      <c r="B10" s="64" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="11"/>
@@ -1917,7 +1918,7 @@
       <c r="R10" s="26">
         <v>49</v>
       </c>
-      <c r="S10" s="41" t="s">
+      <c r="S10" s="40" t="s">
         <v>72</v>
       </c>
       <c r="T10" s="26" t="s">
@@ -1938,7 +1939,7 @@
       <c r="Y10" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="41" t="s">
+      <c r="Z10" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA10" s="26" t="s">
@@ -1959,7 +1960,7 @@
       <c r="AF10" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="AG10" s="41" t="s">
+      <c r="AG10" s="40" t="s">
         <v>73</v>
       </c>
       <c r="AH10" s="26" t="s">
@@ -1980,13 +1981,13 @@
       <c r="AM10" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="AN10" s="45" t="s">
+      <c r="AN10" s="44" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:41" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="62"/>
-      <c r="B11" s="78" t="s">
+      <c r="A11" s="53"/>
+      <c r="B11" s="64" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1994,8 +1995,8 @@
       </c>
     </row>
     <row r="12" spans="1:41" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
-      <c r="B12" s="79" t="s">
+      <c r="A12" s="54"/>
+      <c r="B12" s="65" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="28"/>
@@ -2014,34 +2015,34 @@
       <c r="P12" s="30"/>
       <c r="Q12" s="29"/>
       <c r="R12" s="29"/>
-      <c r="S12" s="42"/>
+      <c r="S12" s="41"/>
       <c r="T12" s="29"/>
       <c r="U12" s="29"/>
       <c r="V12" s="29"/>
       <c r="W12" s="29"/>
       <c r="X12" s="29"/>
       <c r="Y12" s="29"/>
-      <c r="Z12" s="42"/>
+      <c r="Z12" s="41"/>
       <c r="AA12" s="29"/>
       <c r="AB12" s="29"/>
       <c r="AC12" s="29"/>
       <c r="AD12" s="29"/>
       <c r="AE12" s="29"/>
       <c r="AF12" s="29"/>
-      <c r="AG12" s="42"/>
+      <c r="AG12" s="41"/>
       <c r="AH12" s="29"/>
       <c r="AI12" s="29"/>
       <c r="AJ12" s="29"/>
       <c r="AK12" s="29"/>
       <c r="AL12" s="29"/>
       <c r="AM12" s="30"/>
-      <c r="AN12" s="47"/>
+      <c r="AN12" s="46"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="31">
         <v>2</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="66" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -2050,7 +2051,7 @@
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="66" t="s">
         <v>85</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -2058,7 +2059,7 @@
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="66" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="11"/>
@@ -2107,7 +2108,7 @@
       <c r="R15" s="26">
         <v>28</v>
       </c>
-      <c r="S15" s="41" t="s">
+      <c r="S15" s="40" t="s">
         <v>87</v>
       </c>
       <c r="T15" s="26" t="s">
@@ -2128,7 +2129,7 @@
       <c r="Y15" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="Z15" s="41" t="s">
+      <c r="Z15" s="40" t="s">
         <v>69</v>
       </c>
       <c r="AA15" s="26" t="s">
@@ -2149,7 +2150,7 @@
       <c r="AF15" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="AG15" s="41" t="s">
+      <c r="AG15" s="40" t="s">
         <v>92</v>
       </c>
       <c r="AH15" s="26" t="s">
@@ -2170,12 +2171,12 @@
       <c r="AM15" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="AN15" s="45" t="s">
+      <c r="AN15" s="44" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="66" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -2183,7 +2184,7 @@
       </c>
     </row>
     <row r="17" spans="1:40" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="67" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="29"/>
@@ -2195,34 +2196,34 @@
       <c r="P17" s="30"/>
       <c r="Q17" s="29"/>
       <c r="R17" s="29"/>
-      <c r="S17" s="42"/>
+      <c r="S17" s="41"/>
       <c r="T17" s="29"/>
       <c r="U17" s="29"/>
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="29"/>
       <c r="Y17" s="29"/>
-      <c r="Z17" s="42"/>
+      <c r="Z17" s="41"/>
       <c r="AA17" s="29"/>
       <c r="AB17" s="29"/>
       <c r="AC17" s="29"/>
       <c r="AD17" s="29"/>
       <c r="AE17" s="29"/>
       <c r="AF17" s="29"/>
-      <c r="AG17" s="42"/>
+      <c r="AG17" s="41"/>
       <c r="AH17" s="29"/>
       <c r="AI17" s="29"/>
       <c r="AJ17" s="29"/>
       <c r="AK17" s="29"/>
       <c r="AL17" s="29"/>
       <c r="AM17" s="30"/>
-      <c r="AN17" s="47"/>
+      <c r="AN17" s="46"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>3</v>
       </c>
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="66" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2230,7 +2231,7 @@
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="66" t="s">
         <v>96</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -2238,13 +2239,124 @@
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="66" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="11"/>
+      <c r="D20" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M20" s="26">
+        <v>20000</v>
+      </c>
+      <c r="N20" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="O20" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="P20" s="27">
+        <v>16000</v>
+      </c>
+      <c r="Q20" s="26">
+        <v>4000</v>
+      </c>
+      <c r="R20" s="26">
+        <v>28</v>
+      </c>
+      <c r="S20" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="T20" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="U20" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="V20" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="W20" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="X20" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y20" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z20" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA20" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB20" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC20" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD20" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE20" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF20" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG20" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH20" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI20" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ20" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK20" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL20" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM20" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN20" s="44" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="21" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="66" t="s">
         <v>98</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -2252,7 +2364,7 @@
       </c>
     </row>
     <row r="22" spans="1:40" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="81" t="s">
+      <c r="B22" s="67" t="s">
         <v>99</v>
       </c>
       <c r="D22" s="29"/>
@@ -2264,63 +2376,154 @@
       <c r="P22" s="30"/>
       <c r="Q22" s="29"/>
       <c r="R22" s="29"/>
-      <c r="S22" s="42"/>
+      <c r="S22" s="41"/>
       <c r="T22" s="29"/>
       <c r="U22" s="29"/>
       <c r="V22" s="29"/>
       <c r="W22" s="29"/>
       <c r="X22" s="29"/>
       <c r="Y22" s="29"/>
-      <c r="Z22" s="42"/>
+      <c r="Z22" s="41"/>
       <c r="AA22" s="29"/>
       <c r="AB22" s="29"/>
       <c r="AC22" s="29"/>
       <c r="AD22" s="29"/>
       <c r="AE22" s="29"/>
       <c r="AF22" s="29"/>
-      <c r="AG22" s="42"/>
+      <c r="AG22" s="41"/>
       <c r="AH22" s="29"/>
       <c r="AI22" s="29"/>
       <c r="AJ22" s="29"/>
       <c r="AK22" s="29"/>
       <c r="AL22" s="29"/>
       <c r="AM22" s="30"/>
-      <c r="AN22" s="47"/>
+      <c r="AN22" s="46"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
+      <c r="A23" s="11">
+        <v>4</v>
+      </c>
+      <c r="B23" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
+      <c r="B24" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="32"/>
+      <c r="B25" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="E25" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J25" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M25" s="26">
+        <v>20000</v>
+      </c>
+      <c r="N25" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="O25" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="P25" s="27">
+        <v>16000</v>
+      </c>
+      <c r="Q25" s="26">
+        <v>4000</v>
+      </c>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="32"/>
-    </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="32"/>
+      <c r="B26" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" s="27"/>
+      <c r="N26" s="12"/>
+    </row>
+    <row r="27" spans="1:40" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="41"/>
+      <c r="AA27" s="29"/>
+      <c r="AB27" s="29"/>
+      <c r="AC27" s="29"/>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="29"/>
+      <c r="AG27" s="41"/>
+      <c r="AH27" s="29"/>
+      <c r="AI27" s="29"/>
+      <c r="AJ27" s="29"/>
+      <c r="AK27" s="29"/>
+      <c r="AL27" s="29"/>
+      <c r="AM27" s="30"/>
+      <c r="AN27" s="46"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
-      <c r="C28" s="32"/>
+      <c r="C28" s="11"/>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
-      <c r="C29" s="32"/>
+      <c r="C29" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2344,10 +2547,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974E9989-1B5F-FF41-9AD2-81024DE4B8DD}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2362,18 +2565,18 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="74" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="75"/>
-      <c r="F1" s="76"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63"/>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>78</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -2427,6 +2630,11 @@
       </c>
       <c r="F4" s="4" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating all things, end of day
</commit_message>
<xml_diff>
--- a/Results /ml_codes_results.xlsx
+++ b/Results /ml_codes_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Results /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584A1E22-5E41-0D49-A25E-893EDE6C5FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41312A8E-2824-4D49-B757-1E6F51C32F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="132">
   <si>
     <t>Negative DES</t>
   </si>
@@ -393,9 +393,6 @@
     <t>0.549618320610687</t>
   </si>
   <si>
-    <t>hidden_layer_sizes = (1000), # 3 layers of 100 neurons each</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 5.532759435785313e-20</t>
   </si>
   <si>
@@ -418,13 +415,28 @@
   </si>
   <si>
     <t>hidden_layer_sizes = (2000),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hidden_layer_sizes = (1000), </t>
+  </si>
+  <si>
+    <t>0.9565</t>
+  </si>
+  <si>
+    <t>0.967</t>
+  </si>
+  <si>
+    <t>0.4880952380952381</t>
+  </si>
+  <si>
+    <t>0.5381679389312977</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -454,6 +466,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -898,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1107,12 +1125,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1434,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06CD785-33B7-3045-A313-C2EB4D15E3B6}">
-  <dimension ref="A1:AO42"/>
+  <dimension ref="A1:AO57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="AM41" sqref="AM41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2674,7 +2696,7 @@
       <c r="A28" s="11">
         <v>5</v>
       </c>
-      <c r="B28" s="79" t="s">
+      <c r="B28" s="80" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -2683,46 +2705,46 @@
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
-      <c r="B29" s="79" t="s">
+      <c r="B29" s="80" t="s">
         <v>106</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="81"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="80" t="s">
         <v>107</v>
       </c>
       <c r="C30" s="11"/>
-      <c r="D30" s="81" t="s">
+      <c r="D30" s="82" t="s">
         <v>108</v>
       </c>
-      <c r="E30" s="79" t="s">
+      <c r="E30" s="80" t="s">
         <v>109</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="81" t="s">
+      <c r="G30" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="H30" s="79" t="s">
+      <c r="H30" s="80" t="s">
         <v>111</v>
       </c>
-      <c r="I30" s="79" t="s">
+      <c r="I30" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="J30" s="81" t="s">
+      <c r="J30" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="K30" s="79" t="s">
+      <c r="K30" s="80" t="s">
         <v>113</v>
       </c>
-      <c r="L30" s="79" t="s">
+      <c r="L30" s="80" t="s">
         <v>51</v>
       </c>
       <c r="M30" s="26">
@@ -2743,13 +2765,13 @@
       <c r="R30" s="26">
         <v>35</v>
       </c>
-      <c r="S30" s="82" t="s">
-        <v>121</v>
-      </c>
-      <c r="T30" s="81" t="s">
+      <c r="S30" s="83" t="s">
+        <v>120</v>
+      </c>
+      <c r="T30" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="U30" s="79" t="s">
+      <c r="U30" s="80" t="s">
         <v>57</v>
       </c>
       <c r="V30" s="26" t="s">
@@ -2764,13 +2786,13 @@
       <c r="Y30" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="Z30" s="82" t="s">
+      <c r="Z30" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="AA30" s="81" t="s">
+      <c r="AA30" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="AB30" s="79" t="s">
+      <c r="AB30" s="80" t="s">
         <v>60</v>
       </c>
       <c r="AC30" s="26" t="s">
@@ -2785,33 +2807,33 @@
       <c r="AF30" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="AG30" s="83" t="s">
+      <c r="AG30" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="AH30" s="81" t="s">
-        <v>122</v>
-      </c>
-      <c r="AI30" s="84" t="s">
+      <c r="AH30" s="82" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI30" s="85" t="s">
         <v>93</v>
       </c>
       <c r="AJ30" s="26" t="s">
         <v>76</v>
       </c>
       <c r="AK30" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="AL30" s="84" t="s">
+        <v>122</v>
+      </c>
+      <c r="AL30" s="85" t="s">
         <v>83</v>
       </c>
       <c r="AM30" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="AN30" s="82" t="s">
-        <v>124</v>
+      <c r="AN30" s="83" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B31" s="79" t="s">
+      <c r="B31" s="80" t="s">
         <v>98</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -2819,7 +2841,7 @@
       </c>
     </row>
     <row r="32" spans="1:40" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="80" t="s">
+      <c r="B32" s="81" t="s">
         <v>99</v>
       </c>
       <c r="D32" s="29"/>
@@ -2867,7 +2889,7 @@
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B34" s="66" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>28</v>
@@ -2882,7 +2904,7 @@
         <v>86</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>52</v>
@@ -2919,6 +2941,75 @@
       </c>
       <c r="Q35" s="26">
         <v>4000</v>
+      </c>
+      <c r="R35" s="26">
+        <v>32</v>
+      </c>
+      <c r="S35" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="T35" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="U35" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="V35" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="W35" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="X35" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y35" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z35" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA35" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB35" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC35" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD35" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE35" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF35" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG35" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH35" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI35" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ35" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK35" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL35" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM35" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN35" s="44" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.2">
@@ -2969,7 +3060,7 @@
       <c r="A38" s="12">
         <v>7</v>
       </c>
-      <c r="B38" s="79" t="s">
+      <c r="B38" s="80" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="11" t="s">
@@ -2977,21 +3068,63 @@
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B39" s="79" t="s">
-        <v>127</v>
+      <c r="B39" s="80" t="s">
+        <v>126</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B40" s="79" t="s">
+      <c r="B40" s="80" t="s">
         <v>107</v>
       </c>
       <c r="C40" s="11"/>
+      <c r="D40" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="L40" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M40" s="26">
+        <v>20000</v>
+      </c>
+      <c r="N40" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="O40" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="P40" s="27">
+        <v>16000</v>
+      </c>
+      <c r="Q40" s="26">
+        <v>4000</v>
+      </c>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B41" s="79" t="s">
+      <c r="B41" s="80" t="s">
         <v>98</v>
       </c>
       <c r="C41" s="11" t="s">
@@ -2999,7 +3132,7 @@
       </c>
     </row>
     <row r="42" spans="1:40" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="80" t="s">
+      <c r="B42" s="81" t="s">
         <v>99</v>
       </c>
       <c r="D42" s="29"/>
@@ -3034,6 +3167,45 @@
       <c r="AM42" s="30"/>
       <c r="AN42" s="46"/>
     </row>
+    <row r="45" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+      <c r="C45" s="79"/>
+    </row>
+    <row r="46" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+      <c r="C46" s="79"/>
+    </row>
+    <row r="47" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+      <c r="C47" s="79"/>
+    </row>
+    <row r="48" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+      <c r="C48" s="79"/>
+    </row>
+    <row r="49" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C49" s="79"/>
+    </row>
+    <row r="50" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C50" s="79"/>
+    </row>
+    <row r="51" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C51" s="79"/>
+    </row>
+    <row r="52" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C52" s="79"/>
+    </row>
+    <row r="53" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C53" s="79"/>
+    </row>
+    <row r="54" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C54" s="79"/>
+    </row>
+    <row r="55" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C55" s="79"/>
+    </row>
+    <row r="56" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C56" s="79"/>
+    </row>
+    <row r="57" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C57" s="79"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A1:A2"/>
@@ -3050,17 +3222,17 @@
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="J7:L7"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974E9989-1B5F-FF41-9AD2-81024DE4B8DD}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3190,16 +3362,27 @@
         <v>35</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="85" t="s">
+      <c r="E7" s="86" t="s">
         <v>92</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change from 1000 neurons to 100
</commit_message>
<xml_diff>
--- a/Results /ml_codes_results.xlsx
+++ b/Results /ml_codes_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Results /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD8937B-0A35-2C4E-B5F7-B1E389B955B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C253DA-E70C-7B49-8B8C-DDCFA0548003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="21600" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
   </bookViews>
   <sheets>
     <sheet name="ml_lenses results" sheetId="1" r:id="rId1"/>
@@ -1784,8 +1784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06CD785-33B7-3045-A313-C2EB4D15E3B6}">
   <dimension ref="A1:AR86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="R60" sqref="R60"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1807,7 +1807,7 @@
     <col min="15" max="15" width="9.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" style="15" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="76.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15" style="26" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.33203125" style="14" bestFit="1" customWidth="1"/>
@@ -1826,7 +1826,7 @@
     <col min="34" max="34" width="10.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="19.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="11.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="19.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11.5" style="14" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="17.83203125" style="14" bestFit="1" customWidth="1"/>

</xml_diff>